<commit_message>
Match All Report SpreadSheets
</commit_message>
<xml_diff>
--- a/public/downloads/Template Files/All Outstanding Expenses report result.xlsx
+++ b/public/downloads/Template Files/All Outstanding Expenses report result.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RMG\Documents\report template\transactions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RMG\Documents\Task\1-26~Excel Link\Template Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98613C04-2005-4A7B-B3E8-8C4DEB8BC85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B4ACDE-BD58-466E-9A50-1EC04F98132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="All Outstanding Expenses report" sheetId="1" r:id="rId1"/>
+    <sheet name="All Outstanding Expenses Report" sheetId="1" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Raw Data'!$A$1:$AA$26</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -738,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -749,7 +749,6 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1212,38 +1211,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{565A7CE8-6923-4BBF-8BD3-DC758348D00A}" name="TbillReport_IgnoreDates_true_IncludePOs_true_IncludeBills_false_IncludeCredits_f" displayName="TbillReport_IgnoreDates_true_IncludePOs_true_IncludeBills_false_IncludeCredits_f" ref="A1:AA26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{565A7CE8-6923-4BBF-8BD3-DC758348D00A}" name="TbillReport_IgnoreDates_true_IncludePOs_true_IncludeBills_false_IncludeCredits_f" displayName="TbillReport_IgnoreDates_true_IncludePOs_true_IncludeBills_false_IncludeCredits_f" ref="A1:AA26" tableType="queryTable" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:AA26" xr:uid="{565A7CE8-6923-4BBF-8BD3-DC758348D00A}"/>
   <tableColumns count="27">
-    <tableColumn id="28" xr3:uid="{33255ED3-CE8B-43EA-ADB9-CF9F90F9EB6D}" uniqueName="28" name="T.ID" queryTableFieldId="1" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{7ABAAEC1-1335-42F6-85F4-9908C23AAA7D}" uniqueName="2" name="T.ContactId" queryTableFieldId="2" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{6D316BBD-B889-46A7-A20C-7CC8C03AC5BF}" uniqueName="3" name="T.GlobalRef" queryTableFieldId="3" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{62C539E0-ED88-46C1-91D0-FFAD7C0961F5}" uniqueName="4" name="T.PurchaseOrderID" queryTableFieldId="4" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{3E2C8301-3D1D-440F-8DD7-7514138F4EB6}" uniqueName="5" name="T.Type" queryTableFieldId="5" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{87B2AC7F-69D8-4E2E-A715-ED27F640EF55}" uniqueName="6" name="T.ClientID" queryTableFieldId="6" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{12B65A7C-5E13-4B71-AEE9-7FBA2027AEE4}" uniqueName="7" name="T.Company" queryTableFieldId="7" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{79F0C9FB-83A2-4A17-9E2D-B1B1BA6E0958}" uniqueName="8" name="T.PrintName" queryTableFieldId="8" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{E3B19314-1B2D-4FD4-A957-0DD94A98D5B8}" uniqueName="9" name="T.BillNumber" queryTableFieldId="9" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{12089C97-73B2-47D0-8C2C-9516E5C0C2DF}" uniqueName="10" name="T.OrderDate" queryTableFieldId="10" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{6775F53F-F59B-45D3-808F-EB66B6E59F98}" uniqueName="11" name="T.Comments" queryTableFieldId="11" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{A315821A-7F53-46FD-B463-1B30DED1AD48}" uniqueName="12" name="T.Contact" queryTableFieldId="12" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{6B4976CD-91E5-4084-81B4-7867855C87BE}" uniqueName="13" name="T.DueDate" queryTableFieldId="13" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{EF2A4B0B-0F9A-45E0-B5EE-5EF0B71C28FC}" uniqueName="14" name="T.ETADate" queryTableFieldId="14" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{9AF7C7AB-E543-4185-BA0B-96D72878A513}" uniqueName="15" name="T.Phone" queryTableFieldId="15" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{A0C9838B-3A0B-44B2-BC1E-C1FF0CC7897F}" uniqueName="16" name="T.Invoiced" queryTableFieldId="16" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{80AA46AA-0E70-40CA-B247-3DAB3C9EEDF2}" uniqueName="17" name="T.IsCredit" queryTableFieldId="17" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{5309D085-6BE4-46A5-8856-1991D98D5D4C}" uniqueName="18" name="T.InvoiceNumber" queryTableFieldId="18" dataDxfId="11"/>
-    <tableColumn id="19" xr3:uid="{65D2DD50-CB16-4DFA-82F7-D147DF36478C}" uniqueName="19" name="T.IsRA" queryTableFieldId="19" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{CAA76348-AB93-4B21-A30A-2283DE4FAB1F}" uniqueName="20" name="T.Deleted" queryTableFieldId="20" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{570D53CF-1556-4ECE-9290-511588B20081}" uniqueName="21" name="T.SalesComments" queryTableFieldId="21" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{C672F760-196C-44E1-AC7F-DCB11DBA1254}" uniqueName="22" name="T.Total Amount (Ex)" queryTableFieldId="22" dataDxfId="7"/>
-    <tableColumn id="23" xr3:uid="{C7F5EBF6-24FC-45EC-9387-55C6B99634F9}" uniqueName="23" name="T.Total Tax" queryTableFieldId="23" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{23C64215-4E2B-4CC5-B71F-1FA00EECCD55}" uniqueName="24" name="T.Total Amount (Inc)" queryTableFieldId="24" dataDxfId="5"/>
-    <tableColumn id="25" xr3:uid="{C741FB8D-2859-47E4-BD31-6C72D89A4124}" uniqueName="25" name="T.Approved" queryTableFieldId="25" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{0FF711D8-369C-4389-9ED5-0BB9A714B5C0}" uniqueName="26" name="T.CreditOrReturn" queryTableFieldId="26" dataDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{0FCB25B7-C185-4CFB-9281-B91574C508E1}" uniqueName="27" name="T.Balance" queryTableFieldId="27" dataDxfId="2"/>
+    <tableColumn id="28" xr3:uid="{33255ED3-CE8B-43EA-ADB9-CF9F90F9EB6D}" uniqueName="28" name="T.ID" queryTableFieldId="1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{7ABAAEC1-1335-42F6-85F4-9908C23AAA7D}" uniqueName="2" name="T.ContactId" queryTableFieldId="2" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{6D316BBD-B889-46A7-A20C-7CC8C03AC5BF}" uniqueName="3" name="T.GlobalRef" queryTableFieldId="3" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{62C539E0-ED88-46C1-91D0-FFAD7C0961F5}" uniqueName="4" name="T.PurchaseOrderID" queryTableFieldId="4" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{3E2C8301-3D1D-440F-8DD7-7514138F4EB6}" uniqueName="5" name="T.Type" queryTableFieldId="5" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{87B2AC7F-69D8-4E2E-A715-ED27F640EF55}" uniqueName="6" name="T.ClientID" queryTableFieldId="6" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{12B65A7C-5E13-4B71-AEE9-7FBA2027AEE4}" uniqueName="7" name="T.Company" queryTableFieldId="7" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{79F0C9FB-83A2-4A17-9E2D-B1B1BA6E0958}" uniqueName="8" name="T.PrintName" queryTableFieldId="8" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{E3B19314-1B2D-4FD4-A957-0DD94A98D5B8}" uniqueName="9" name="T.BillNumber" queryTableFieldId="9" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{12089C97-73B2-47D0-8C2C-9516E5C0C2DF}" uniqueName="10" name="T.OrderDate" queryTableFieldId="10" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{6775F53F-F59B-45D3-808F-EB66B6E59F98}" uniqueName="11" name="T.Comments" queryTableFieldId="11" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{A315821A-7F53-46FD-B463-1B30DED1AD48}" uniqueName="12" name="T.Contact" queryTableFieldId="12" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{6B4976CD-91E5-4084-81B4-7867855C87BE}" uniqueName="13" name="T.DueDate" queryTableFieldId="13" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{EF2A4B0B-0F9A-45E0-B5EE-5EF0B71C28FC}" uniqueName="14" name="T.ETADate" queryTableFieldId="14" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{9AF7C7AB-E543-4185-BA0B-96D72878A513}" uniqueName="15" name="T.Phone" queryTableFieldId="15" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{A0C9838B-3A0B-44B2-BC1E-C1FF0CC7897F}" uniqueName="16" name="T.Invoiced" queryTableFieldId="16" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{80AA46AA-0E70-40CA-B247-3DAB3C9EEDF2}" uniqueName="17" name="T.IsCredit" queryTableFieldId="17" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{5309D085-6BE4-46A5-8856-1991D98D5D4C}" uniqueName="18" name="T.InvoiceNumber" queryTableFieldId="18" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{65D2DD50-CB16-4DFA-82F7-D147DF36478C}" uniqueName="19" name="T.IsRA" queryTableFieldId="19" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{CAA76348-AB93-4B21-A30A-2283DE4FAB1F}" uniqueName="20" name="T.Deleted" queryTableFieldId="20" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{570D53CF-1556-4ECE-9290-511588B20081}" uniqueName="21" name="T.SalesComments" queryTableFieldId="21" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{C672F760-196C-44E1-AC7F-DCB11DBA1254}" uniqueName="22" name="T.Total Amount (Ex)" queryTableFieldId="22" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{C7F5EBF6-24FC-45EC-9387-55C6B99634F9}" uniqueName="23" name="T.Total Tax" queryTableFieldId="23" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{23C64215-4E2B-4CC5-B71F-1FA00EECCD55}" uniqueName="24" name="T.Total Amount (Inc)" queryTableFieldId="24" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{C741FB8D-2859-47E4-BD31-6C72D89A4124}" uniqueName="25" name="T.Approved" queryTableFieldId="25" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{0FF711D8-369C-4389-9ED5-0BB9A714B5C0}" uniqueName="26" name="T.CreditOrReturn" queryTableFieldId="26" dataDxfId="1"/>
+    <tableColumn id="27" xr3:uid="{0FCB25B7-C185-4CFB-9281-B91574C508E1}" uniqueName="27" name="T.Balance" queryTableFieldId="27" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1512,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,38 +2235,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A56D334-305E-4050-8DCE-17ED13D17784}">
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AA26"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21:N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
@@ -2852,1579 +2850,1579 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>82</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>44</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M8" s="5" t="s">
+      <c r="L8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="O8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="5" t="b">
+      <c r="O8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" s="5" t="s">
+      <c r="Q8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="S8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V8" s="5">
+      <c r="S8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V8" s="4">
         <v>8271</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8" s="4">
         <v>1240.6500000000001</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="4">
         <v>9511.65</v>
       </c>
-      <c r="Y8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA8" s="5">
+      <c r="Y8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA8" s="4">
         <v>9511.65</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>93</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>56</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M9" s="5" t="s">
+      <c r="L9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P9" s="5" t="b">
+      <c r="P9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" s="5" t="s">
+      <c r="Q9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="S9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U9" s="5" t="s">
+      <c r="S9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="4">
         <v>2400</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9" s="4">
         <v>360</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="4">
         <v>2760</v>
       </c>
-      <c r="Y9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA9" s="5">
+      <c r="Y9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA9" s="4">
         <v>2760</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>101</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>56</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M10" s="5" t="s">
+      <c r="K10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="5" t="b">
+      <c r="P10" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" s="5" t="s">
+      <c r="Q10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="S10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V10" s="5">
+      <c r="S10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10" s="4">
         <v>80</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="4">
         <v>12</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="4">
         <v>92</v>
       </c>
-      <c r="Y10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA10" s="5">
+      <c r="Y10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA10" s="4">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>108</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>56</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M11" s="5" t="s">
+      <c r="K11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P11" s="5" t="b">
+      <c r="P11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5" t="s">
+      <c r="Q11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="S11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U11" s="5" t="s">
+      <c r="S11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="4">
         <v>800</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11" s="4">
         <v>120</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X11" s="4">
         <v>920</v>
       </c>
-      <c r="Y11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA11" s="5">
+      <c r="Y11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA11" s="4">
         <v>920</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>109</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>41</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M12" s="5" t="s">
+      <c r="K12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="O12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P12" s="5" t="b">
+      <c r="O12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V12" s="5">
+      <c r="Q12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V12" s="4">
         <v>800</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="4">
         <v>120</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="4">
         <v>920</v>
       </c>
-      <c r="Y12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA12" s="5">
+      <c r="Y12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA12" s="4">
         <v>920</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>110</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>103</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13" s="5" t="s">
+      <c r="K13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="P13" s="5" t="b">
+      <c r="P13" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U13" s="5" t="s">
+      <c r="Q13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="4">
         <v>1200</v>
       </c>
-      <c r="W13" s="5">
+      <c r="W13" s="4">
         <v>180</v>
       </c>
-      <c r="X13" s="5">
+      <c r="X13" s="4">
         <v>1380</v>
       </c>
-      <c r="Y13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA13" s="5">
+      <c r="Y13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA13" s="4">
         <v>1380</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>115</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>55</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M14" s="5" t="s">
+      <c r="L14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P14" s="5" t="b">
+      <c r="P14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R14" s="5" t="s">
+      <c r="Q14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="S14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V14" s="5">
+      <c r="S14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V14" s="4">
         <v>250000</v>
       </c>
-      <c r="W14" s="5">
-        <v>0</v>
-      </c>
-      <c r="X14" s="5">
+      <c r="W14" s="4">
+        <v>0</v>
+      </c>
+      <c r="X14" s="4">
         <v>250000</v>
       </c>
-      <c r="Y14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA14" s="5">
+      <c r="Y14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA14" s="4">
         <v>250000</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="A15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>119</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>60</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M15" s="5" t="s">
+      <c r="K15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="P15" s="5" t="b">
+      <c r="P15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R15" s="5" t="s">
+      <c r="Q15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="S15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V15" s="5">
+      <c r="S15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V15" s="4">
         <v>50</v>
       </c>
-      <c r="W15" s="5">
-        <v>0</v>
-      </c>
-      <c r="X15" s="5">
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
         <v>50</v>
       </c>
-      <c r="Y15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA15" s="5">
+      <c r="Y15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA15" s="4">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="A16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>124</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>56</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" s="5" t="s">
+      <c r="L16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P16" s="5" t="b">
+      <c r="P16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R16" s="5" t="s">
+      <c r="Q16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="S16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U16" s="5" t="s">
+      <c r="S16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="V16" s="5">
+      <c r="V16" s="4">
         <v>20</v>
       </c>
-      <c r="W16" s="5">
+      <c r="W16" s="4">
         <v>4</v>
       </c>
-      <c r="X16" s="5">
+      <c r="X16" s="4">
         <v>24</v>
       </c>
-      <c r="Y16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA16" s="5">
+      <c r="Y16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA16" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>125</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>56</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M17" s="5" t="s">
+      <c r="L17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="O17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P17" s="5" t="b">
+      <c r="P17" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R17" s="5" t="s">
+      <c r="Q17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="S17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U17" s="5" t="s">
+      <c r="S17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="V17" s="5">
+      <c r="V17" s="4">
         <v>20</v>
       </c>
-      <c r="W17" s="5">
+      <c r="W17" s="4">
         <v>4</v>
       </c>
-      <c r="X17" s="5">
+      <c r="X17" s="4">
         <v>24</v>
       </c>
-      <c r="Y17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA17" s="5">
+      <c r="Y17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA17" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>126</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>103</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M18" s="5" t="s">
+      <c r="K18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="O18" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="P18" s="5" t="b">
+      <c r="P18" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R18" s="5" t="s">
+      <c r="Q18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="S18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V18" s="5">
+      <c r="S18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V18" s="4">
         <v>20</v>
       </c>
-      <c r="W18" s="5">
+      <c r="W18" s="4">
         <v>4</v>
       </c>
-      <c r="X18" s="5">
+      <c r="X18" s="4">
         <v>24</v>
       </c>
-      <c r="Y18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA18" s="5">
+      <c r="Y18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA18" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="A19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>127</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>103</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M19" s="5" t="s">
+      <c r="L19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="O19" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="P19" s="5" t="b">
+      <c r="P19" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R19" s="5" t="s">
+      <c r="Q19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="S19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U19" s="5" t="s">
+      <c r="S19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="V19" s="5">
+      <c r="V19" s="4">
         <v>20</v>
       </c>
-      <c r="W19" s="5">
+      <c r="W19" s="4">
         <v>4</v>
       </c>
-      <c r="X19" s="5">
+      <c r="X19" s="4">
         <v>24</v>
       </c>
-      <c r="Y19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA19" s="5">
+      <c r="Y19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA19" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="5">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="A20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>130</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>56</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M20" s="5" t="s">
+      <c r="K20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="O20" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="5" t="b">
+      <c r="P20" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R20" s="5" t="s">
+      <c r="Q20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="S20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V20" s="5">
+      <c r="S20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V20" s="4">
         <v>8</v>
       </c>
-      <c r="W20" s="5">
+      <c r="W20" s="4">
         <v>1.2</v>
       </c>
-      <c r="X20" s="5">
+      <c r="X20" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="Y20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA20" s="5">
+      <c r="Y20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA20" s="4">
         <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="5">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="A21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>131</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>56</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M21" s="5" t="s">
+      <c r="K21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="O21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P21" s="5" t="b">
+      <c r="P21" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R21" s="5" t="s">
+      <c r="Q21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="S21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V21" s="5">
+      <c r="S21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V21" s="4">
         <v>8</v>
       </c>
-      <c r="W21" s="5">
+      <c r="W21" s="4">
         <v>1.2</v>
       </c>
-      <c r="X21" s="5">
+      <c r="X21" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="Y21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA21" s="5">
+      <c r="Y21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA21" s="4">
         <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="5">
-        <v>0</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>133</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>56</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M22" s="5" t="s">
+      <c r="L22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M22" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="O22" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P22" s="5" t="b">
+      <c r="P22" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R22" s="5" t="s">
+      <c r="Q22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="S22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U22" s="5" t="s">
+      <c r="S22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="V22" s="5">
+      <c r="V22" s="4">
         <v>800</v>
       </c>
-      <c r="W22" s="5">
+      <c r="W22" s="4">
         <v>120</v>
       </c>
-      <c r="X22" s="5">
+      <c r="X22" s="4">
         <v>920</v>
       </c>
-      <c r="Y22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA22" s="5">
+      <c r="Y22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA22" s="4">
         <v>920</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="A23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>146</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>56</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M23" s="5" t="s">
+      <c r="K23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="O23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P23" s="5" t="b">
+      <c r="P23" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R23" s="5" t="s">
+      <c r="Q23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="S23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V23" s="5">
+      <c r="S23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V23" s="4">
         <v>800</v>
       </c>
-      <c r="W23" s="5">
+      <c r="W23" s="4">
         <v>120</v>
       </c>
-      <c r="X23" s="5">
+      <c r="X23" s="4">
         <v>920</v>
       </c>
-      <c r="Y23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA23" s="5">
+      <c r="Y23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA23" s="4">
         <v>920</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="A24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>147</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>79</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M24" s="5" t="s">
+      <c r="K24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="O24" s="5" t="s">
+      <c r="O24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="P24" s="5" t="b">
+      <c r="P24" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R24" s="5" t="s">
+      <c r="Q24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="S24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V24" s="5">
+      <c r="S24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V24" s="4">
         <v>47</v>
       </c>
-      <c r="W24" s="5">
+      <c r="W24" s="4">
         <v>7.05</v>
       </c>
-      <c r="X24" s="5">
+      <c r="X24" s="4">
         <v>54.05</v>
       </c>
-      <c r="Y24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA24" s="5">
+      <c r="Y24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA24" s="4">
         <v>54.05</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="A25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>179</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>142</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M25" s="5" t="s">
+      <c r="K25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="P25" s="5" t="b">
+      <c r="P25" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R25" s="5" t="s">
+      <c r="Q25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="S25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V25" s="5">
+      <c r="S25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V25" s="4">
         <v>5</v>
       </c>
-      <c r="W25" s="5">
-        <v>0</v>
-      </c>
-      <c r="X25" s="5">
+      <c r="W25" s="4">
+        <v>0</v>
+      </c>
+      <c r="X25" s="4">
         <v>5</v>
       </c>
-      <c r="Y25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA25" s="5">
+      <c r="Y25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA25" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="5">
-        <v>0</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="A26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>224</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>103</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M26" s="5" t="s">
+      <c r="K26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="O26" s="5" t="s">
+      <c r="O26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="P26" s="5" t="b">
+      <c r="P26" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V26" s="5">
+      <c r="Q26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V26" s="4">
         <v>400</v>
       </c>
-      <c r="W26" s="5">
+      <c r="W26" s="4">
         <v>60</v>
       </c>
-      <c r="X26" s="5">
+      <c r="X26" s="4">
         <v>460</v>
       </c>
-      <c r="Y26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA26" s="5">
+      <c r="Y26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA26" s="4">
         <v>460</v>
       </c>
     </row>

</xml_diff>